<commit_message>
update fitur reset role admin
</commit_message>
<xml_diff>
--- a/admin/uploads/data_ppdb_sd_tes_importdata.xlsx
+++ b/admin/uploads/data_ppdb_sd_tes_importdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\format excel import data siswa aplikasi daily\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02F5320-5672-4F6F-B020-C87F5D7E5C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D008784-9F61-4A59-B0B9-F6868875DEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="617">
   <si>
     <t>pendaftaran_kelas</t>
   </si>
@@ -2772,8 +2772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BD10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BL11" sqref="BL11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5413,8 +5413,8 @@
       <c r="BG14" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="BH14" s="6" t="s">
-        <v>177</v>
+      <c r="BH14" s="6">
+        <v>45614.579050925924</v>
       </c>
       <c r="BI14" s="2">
         <v>202502007</v>

</xml_diff>